<commit_message>
Added excel-in and excel-out tags
</commit_message>
<xml_diff>
--- a/test/export_employees.xlsx
+++ b/test/export_employees.xlsx
@@ -55,12 +55,12 @@
     <t>test@test.com</t>
   </si>
   <si>
+    <t>05/10/2022</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>[]</t>
-  </si>
-  <si>
     <t>{"first_name":"","last_name":"","full_name":""}</t>
   </si>
   <si>
@@ -73,7 +73,7 @@
     <t>anonymous</t>
   </si>
   <si>
-    <t>[1 2]</t>
+    <t>1;2</t>
   </si>
 </sst>
 </file>
@@ -108,11 +108,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="false">
-      <alignment/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,14 +428,12 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
+      <c r="E2" t="str"/>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="1">
-        <v>44838.452805625704</v>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -460,17 +455,13 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
+      <c r="D3" t="str"/>
+      <c r="E3" t="str"/>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -492,17 +483,13 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
+      <c r="D4" t="str"/>
+      <c r="E4" t="str"/>
       <c r="F4">
         <v>32</v>
       </c>
-      <c r="G4" s="1">
-        <v>44838.452805625704</v>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
       <c r="H4">
         <v>0</v>

</xml_diff>

<commit_message>
go 1.20 + modules update
</commit_message>
<xml_diff>
--- a/test/export_employees.xlsx
+++ b/test/export_employees.xlsx
@@ -55,7 +55,7 @@
     <t>test@test.com</t>
   </si>
   <si>
-    <t>05/10/2022</t>
+    <t>03/02/2023</t>
   </si>
   <si>
     <t/>
@@ -120,120 +120,120 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
+<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <themeElements>
+    <clrScheme name="Office">
+      <dk1>
+        <sysClr val="windowText" lastClr="000000"/>
+      </dk1>
+      <lt1>
+        <sysClr val="window" lastClr="FFFFFF"/>
+      </lt1>
+      <dk2>
+        <srgbClr val="44546A"/>
+      </dk2>
+      <lt2>
+        <srgbClr val="E7E6E6"/>
+      </lt2>
+      <accent1>
+        <srgbClr val="5B9BD5"/>
+      </accent1>
+      <accent2>
+        <srgbClr val="ED7D31"/>
+      </accent2>
+      <accent3>
+        <srgbClr val="A5A5A5"/>
+      </accent3>
+      <accent4>
+        <srgbClr val="FFC000"/>
+      </accent4>
+      <accent5>
+        <srgbClr val="4472C4"/>
+      </accent5>
+      <accent6>
+        <srgbClr val="70AD47"/>
+      </accent6>
+      <hlink>
+        <srgbClr val="0563C1"/>
+      </hlink>
+      <folHlink>
+        <srgbClr val="954F72"/>
+      </folHlink>
+    </clrScheme>
+    <fontScheme name="Office">
+      <majorFont>
+        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック Light"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线 Light"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Times New Roman"/>
+        <font script="Hebr" typeface="Times New Roman"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="MoolBoran"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Times New Roman"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </majorFont>
+      <minorFont>
+        <latin typeface="Calibri" panose="020F0502020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Arial"/>
+        <font script="Hebr" typeface="Arial"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="DaunPenh"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Arial"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </minorFont>
+    </fontScheme>
+    <fmtScheme name="Office">
+      <fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -289,8 +289,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
+      </fillStyleLst>
+      <lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -312,8 +312,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
+      </lnStyleLst>
+      <effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -329,8 +329,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
+      </effectStyleLst>
+      <bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -367,12 +367,12 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
+      </bgFillStyleLst>
+    </fmtScheme>
+  </themeElements>
+  <objectDefaults/>
+  <extraClrSchemeLst/>
+</theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,7 +428,6 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="str"/>
       <c r="F2">
         <v>0</v>
       </c>
@@ -455,8 +454,6 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="str"/>
-      <c r="E3" t="str"/>
       <c r="F3">
         <v>0</v>
       </c>
@@ -483,8 +480,6 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="str"/>
-      <c r="E4" t="str"/>
       <c r="F4">
         <v>32</v>
       </c>

</xml_diff>